<commit_message>
Add all text to application section. Table references need to be fixed. Small edits otherwise.
Former-commit-id: 605dab0a8503eb0d4e92b5de959cc1dcea1821ca
</commit_message>
<xml_diff>
--- a/images/author_summary.xlsx
+++ b/images/author_summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbarnes/Documents/GitHub/resiliency_paper/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{068721AF-0339-AD48-89B3-4C7CC671781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3099FE44-20A2-D347-A4BD-5F2C8412182E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="author_summary" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -965,14 +965,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Fix a couple of more issues with building the previous document
</commit_message>
<xml_diff>
--- a/images/author_summary.xlsx
+++ b/images/author_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbarnes/Documents/GitHub/resiliency_paper/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregmacfarlane/projects/resiliency_paper/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3099FE44-20A2-D347-A4BD-5F2C8412182E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F05AB-E847-7048-B46D-1192E7E46CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="21240" windowWidth="38400" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="author_summary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Year</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t>Hackl and Adey</t>
+  </si>
+  <si>
+    <t>Taylor and Susilawati</t>
+  </si>
+  <si>
+    <t>Gecchele et al.</t>
+  </si>
+  <si>
+    <t>Scott et al.</t>
+  </si>
+  <si>
+    <t>Jenelius and Mattson</t>
+  </si>
+  <si>
+    <t>Balijepalli and Oppong</t>
   </si>
 </sst>
 </file>
@@ -605,12 +620,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -670,9 +684,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -710,7 +724,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -816,7 +830,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -958,7 +972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -966,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,7 +992,7 @@
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,9 +1002,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2004</v>
       </c>
@@ -1000,259 +1013,292 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2007</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>2008</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2010</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2010</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2010</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2011</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2011</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>2013</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>2014</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>2015</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>